<commit_message>
zasady ustalone i bawienei sie ekraniem z pytaniami
</commit_message>
<xml_diff>
--- a/data_base/PytaniaProjekt.xlsx
+++ b/data_base/PytaniaProjekt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damia\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damia\Desktop\Trivia_Game\data_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02C33CFC-32A6-4D5D-B5FE-FA22EBAA76AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611A1A5C-47C3-4901-B6DD-4FB9B0973135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{6141DBD3-99C8-4C1A-8268-ADC8A4714638}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6141DBD3-99C8-4C1A-8268-ADC8A4714638}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>pytanie</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>odpowiedz poprawna</t>
   </si>
@@ -39,22 +36,25 @@
     <t>odpowiedz3</t>
   </si>
   <si>
-    <t>odpowiedz4</t>
-  </si>
-  <si>
     <t>kategoria</t>
   </si>
   <si>
-    <t>czy było już</t>
-  </si>
-  <si>
     <t>sport</t>
   </si>
   <si>
-    <t>jaki był wynik meczu blabla</t>
-  </si>
-  <si>
-    <t>false</t>
+    <t>1:1</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>W jakim klubie gra Robert Lewandowski?</t>
+  </si>
+  <si>
+    <t>pytanie (max 80 znakow)</t>
+  </si>
+  <si>
+    <t>max 26 znakow odpowiedzi</t>
   </si>
 </sst>
 </file>
@@ -71,12 +71,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -106,10 +112,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -424,67 +434,410 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE2B563-E523-4F70-9BE4-817456DC8DAD}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="2">
+        <v>4.2361111111111106E-2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>8.5416666666666655E-2</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="C2" s="2">
-        <v>8.4027777777777771E-2</v>
-      </c>
-      <c r="D2" s="2">
-        <v>4.2361111111111106E-2</v>
-      </c>
-      <c r="E2" s="2">
-        <v>8.5416666666666655E-2</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>9</v>
       </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>